<commit_message>
clean app and outsource the manual
</commit_message>
<xml_diff>
--- a/www/BCA_assay_OT2_96well_half_area_template.xlsx
+++ b/www/BCA_assay_OT2_96well_half_area_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/shinyBCA_PlateReader/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/MassSpecPreppy/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8FB678-8E7D-5C41-B353-96F9B3050616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63391605-8A05-924E-8E36-BF09406C3E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="2720" windowWidth="28040" windowHeight="17440" xr2:uid="{DBEC7D3F-F76B-FF4C-B0AF-4D248AC37558}"/>
+    <workbookView xWindow="20600" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{DBEC7D3F-F76B-FF4C-B0AF-4D248AC37558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -146,13 +146,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -167,8 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,348 +514,350 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="C35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="C36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="C40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="C41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing deck layout bug when using e.g. multiple dilutions per sample in BCA assay or multiple sample preparations from a single sample
</commit_message>
<xml_diff>
--- a/www/BCA_assay_OT2_96well_half_area_template.xlsx
+++ b/www/BCA_assay_OT2_96well_half_area_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/MassSpecPreppy/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63391605-8A05-924E-8E36-BF09406C3E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460EAB66-823E-6740-8369-4908801E9C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20600" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{DBEC7D3F-F76B-FF4C-B0AF-4D248AC37558}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>dilution</t>
   </si>
   <si>
-    <t>OT-2 plate</t>
-  </si>
-  <si>
     <t>OT-2 position</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>sample_volume</t>
+  </si>
+  <si>
+    <t>OT-2 slot</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,333 +532,333 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
polish BCA assay OT2 download columns names and move python file
</commit_message>
<xml_diff>
--- a/www/BCA_assay_OT2_96well_half_area_template.xlsx
+++ b/www/BCA_assay_OT2_96well_half_area_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/MassSpecPreppy/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460EAB66-823E-6740-8369-4908801E9C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D049BDA1-4388-0D48-8247-6E4320C49470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20600" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{DBEC7D3F-F76B-FF4C-B0AF-4D248AC37558}"/>
   </bookViews>
@@ -38,9 +38,6 @@
     <t>sample</t>
   </si>
   <si>
-    <t>dilution</t>
-  </si>
-  <si>
     <t>OT-2 position</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>OT-2 slot</t>
+  </si>
+  <si>
+    <t>x-fold dilution</t>
   </si>
 </sst>
 </file>
@@ -192,11 +192,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +519,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,341 +529,341 @@
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- bugfixes - implementation of BCA assay dilutions down to 5x - improve BCA assay OT-2 template generation UI response - add 20µl tiüps used in decklayout plot for BCA assay - add shiny alerts for BCA assay template generation
</commit_message>
<xml_diff>
--- a/www/BCA_assay_OT2_96well_half_area_template.xlsx
+++ b/www/BCA_assay_OT2_96well_half_area_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/Shiny_Projects/MassSpecPreppy/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephanmichalik/Desktop/MassSpecPreppy/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D049BDA1-4388-0D48-8247-6E4320C49470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F27A39-335F-9A4C-9DAD-480DB96C6DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20600" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{DBEC7D3F-F76B-FF4C-B0AF-4D248AC37558}"/>
+    <workbookView xWindow="34560" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{DBEC7D3F-F76B-FF4C-B0AF-4D248AC37558}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -119,20 +111,20 @@
     <t>D6</t>
   </si>
   <si>
-    <t>sample_volume</t>
-  </si>
-  <si>
     <t>OT-2 slot</t>
   </si>
   <si>
     <t>x-fold dilution</t>
+  </si>
+  <si>
+    <t>volume (µl)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +139,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -192,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -200,6 +200,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -519,7 +522,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,16 +537,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>28</v>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>